<commit_message>
worked on contacts bulk upload and viewing on ace profile
</commit_message>
<xml_diff>
--- a/public/Contacts/contacts.xlsx
+++ b/public/Contacts/contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faith Kilonzi\Documents\ace-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB590FC-716C-4BC7-BAB8-6E081851D534}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3726658-7211-44AF-8677-DB31C4DB7C3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6C807407-21A2-43CE-AE5B-37A99DD9C75B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Position</t>
   </si>
@@ -81,15 +81,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>joseph.mensah@gmail.com</t>
-  </si>
-  <si>
-    <t>Kenya</t>
-  </si>
-  <si>
-    <t>Angola</t>
-  </si>
-  <si>
     <t>Ghana</t>
   </si>
   <si>
@@ -105,9 +96,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>University of Ghana</t>
-  </si>
-  <si>
     <t>Kofinuel Emmanuel</t>
   </si>
   <si>
@@ -123,34 +111,43 @@
     <t>George KuntaKunta</t>
   </si>
   <si>
-    <t>georgie@gmail.com</t>
-  </si>
-  <si>
-    <t>enyonamh@gmail.com</t>
-  </si>
-  <si>
-    <t>maryjaneh@gmail.com</t>
-  </si>
-  <si>
-    <t>njorogek@gmail.com</t>
-  </si>
-  <si>
-    <t>kofinuel@gmail.com</t>
-  </si>
-  <si>
-    <t>CDA</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Agriculture</t>
-  </si>
-  <si>
     <t>Focal Point person</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>jmesnah@gmail.com</t>
+  </si>
+  <si>
+    <t>kariukij@gmail.com</t>
+  </si>
+  <si>
+    <t>emamnuel@gmail.com</t>
+  </si>
+  <si>
+    <t>janemama@gmail.com</t>
+  </si>
+  <si>
+    <t>etonammensah@gmail.com</t>
+  </si>
+  <si>
+    <t>georgiekuntae@gmail.com</t>
+  </si>
+  <si>
+    <t>MS4SSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Université Abdou Moumouni	</t>
+  </si>
+  <si>
+    <t>Niger</t>
   </si>
 </sst>
 </file>
@@ -524,7 +521,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,24 +590,24 @@
         <v>24560223058</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
       <c r="L2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -619,13 +616,13 @@
         <v>24560223058</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="L3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -636,7 +633,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -645,76 +642,76 @@
         <v>24560223058</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="L4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F5">
         <v>24560223058</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>24560223058</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="L6" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -723,13 +720,13 @@
         <v>24560223058</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>